<commit_message>
added species of local concern
</commit_message>
<xml_diff>
--- a/output/manual_range_edge_binning.xlsx
+++ b/output/manual_range_edge_binning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usdagcc.sharepoint.com/sites/fs-cio-mpsg/SCC Library/03_Nebraska NFG/Species Evaluations/R_NNFG_SO/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1850" documentId="11_70DE90B082F123B351BBEF595328C939760EC9C2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04BEFA66-B841-4C70-84B9-BE9CE0DB60FB}"/>
+  <xr:revisionPtr revIDLastSave="1858" documentId="11_70DE90B082F123B351BBEF595328C939760EC9C2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A1BB6D9-D40C-4523-8D91-590C010E894F}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bins" sheetId="1" r:id="rId1"/>
@@ -3007,7 +3007,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3524,7 +3524,10 @@
   <autoFilter ref="A1:S230" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}">
     <filterColumn colId="2">
       <filters>
+        <filter val="Autumnal Water-starwort"/>
+        <filter val="Graham's Rockcress"/>
         <filter val="Pearly Everlasting"/>
+        <filter val="Vernal Water-starwort"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3835,18 +3838,18 @@
   <dimension ref="A1:S230"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K112" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="R163" sqref="R163"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D125" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="I239" sqref="I239"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" style="4" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="4" customWidth="1"/>
     <col min="3" max="3" width="26.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="4" customWidth="1"/>
     <col min="5" max="5" width="6.5703125" style="4" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" style="4" customWidth="1"/>
     <col min="7" max="7" width="5.42578125" style="4" customWidth="1"/>
@@ -3865,7 +3868,7 @@
     <col min="20" max="16384" width="11.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="30">
+    <row r="1" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3924,7 +3927,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="45" hidden="1">
+    <row r="2" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>19</v>
       </c>
@@ -3969,7 +3972,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="30" hidden="1">
+    <row r="3" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>33</v>
       </c>
@@ -4014,7 +4017,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="30" hidden="1">
+    <row r="4" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>38</v>
       </c>
@@ -4067,7 +4070,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="75" hidden="1">
+    <row r="5" spans="1:19" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>50</v>
       </c>
@@ -4108,7 +4111,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="45" hidden="1">
+    <row r="6" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>57</v>
       </c>
@@ -4159,7 +4162,7 @@
       </c>
       <c r="S6" s="5"/>
     </row>
-    <row r="7" spans="1:19" ht="60" hidden="1">
+    <row r="7" spans="1:19" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>64</v>
       </c>
@@ -4212,7 +4215,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="30" hidden="1">
+    <row r="8" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>72</v>
       </c>
@@ -4265,7 +4268,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="45" hidden="1">
+    <row r="9" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>79</v>
       </c>
@@ -4315,7 +4318,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="30" hidden="1">
+    <row r="10" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>83</v>
       </c>
@@ -4368,7 +4371,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="45" hidden="1">
+    <row r="11" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>89</v>
       </c>
@@ -4421,7 +4424,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="45" hidden="1">
+    <row r="12" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>93</v>
       </c>
@@ -4474,7 +4477,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="45" hidden="1">
+    <row r="13" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>98</v>
       </c>
@@ -4515,7 +4518,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="30" hidden="1">
+    <row r="14" spans="1:19" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>104</v>
       </c>
@@ -4568,7 +4571,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="45" hidden="1">
+    <row r="15" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>112</v>
       </c>
@@ -4621,7 +4624,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="60" hidden="1">
+    <row r="16" spans="1:19" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>116</v>
       </c>
@@ -4674,7 +4677,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="30" hidden="1">
+    <row r="17" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>120</v>
       </c>
@@ -4727,7 +4730,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="45" hidden="1">
+    <row r="18" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>125</v>
       </c>
@@ -4780,7 +4783,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="45" hidden="1">
+    <row r="19" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>130</v>
       </c>
@@ -4821,7 +4824,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="45" hidden="1">
+    <row r="20" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>134</v>
       </c>
@@ -4874,7 +4877,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="45" hidden="1">
+    <row r="21" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>138</v>
       </c>
@@ -4927,7 +4930,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="30" hidden="1">
+    <row r="22" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>144</v>
       </c>
@@ -4968,7 +4971,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="30" hidden="1">
+    <row r="23" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>149</v>
       </c>
@@ -5018,7 +5021,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="60" hidden="1">
+    <row r="24" spans="1:18" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>153</v>
       </c>
@@ -5071,7 +5074,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="30" hidden="1">
+    <row r="25" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>160</v>
       </c>
@@ -5124,7 +5127,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="30" hidden="1">
+    <row r="26" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>167</v>
       </c>
@@ -5177,7 +5180,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="60" hidden="1">
+    <row r="27" spans="1:18" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>171</v>
       </c>
@@ -5230,7 +5233,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="60" hidden="1">
+    <row r="28" spans="1:18" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>176</v>
       </c>
@@ -5283,7 +5286,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="70.5" hidden="1" customHeight="1">
+    <row r="29" spans="1:18" ht="70.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>180</v>
       </c>
@@ -5333,7 +5336,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="45" hidden="1">
+    <row r="30" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>184</v>
       </c>
@@ -5374,7 +5377,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="30" hidden="1">
+    <row r="31" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>188</v>
       </c>
@@ -5427,7 +5430,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="45" hidden="1">
+    <row r="32" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>192</v>
       </c>
@@ -5480,7 +5483,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="30" hidden="1">
+    <row r="33" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>199</v>
       </c>
@@ -5533,7 +5536,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="45" hidden="1">
+    <row r="34" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>203</v>
       </c>
@@ -5583,7 +5586,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="45" hidden="1">
+    <row r="35" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>206</v>
       </c>
@@ -5636,7 +5639,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="45" hidden="1">
+    <row r="36" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>211</v>
       </c>
@@ -5689,7 +5692,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="45" hidden="1">
+    <row r="37" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>216</v>
       </c>
@@ -5739,7 +5742,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="45" hidden="1">
+    <row r="38" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>219</v>
       </c>
@@ -5792,7 +5795,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="45" hidden="1">
+    <row r="39" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>224</v>
       </c>
@@ -5845,7 +5848,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="40" spans="1:18" ht="61.5" hidden="1" customHeight="1">
+    <row r="40" spans="1:18" ht="61.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>228</v>
       </c>
@@ -5898,7 +5901,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="37.5" hidden="1" customHeight="1">
+    <row r="41" spans="1:18" ht="37.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>232</v>
       </c>
@@ -5951,7 +5954,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="45" hidden="1">
+    <row r="42" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>236</v>
       </c>
@@ -6004,7 +6007,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="60" hidden="1" customHeight="1">
+    <row r="43" spans="1:18" ht="60" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>240</v>
       </c>
@@ -6057,7 +6060,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="45" hidden="1">
+    <row r="44" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>244</v>
       </c>
@@ -6110,7 +6113,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="45" spans="1:18" ht="30" hidden="1">
+    <row r="45" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>249</v>
       </c>
@@ -6155,7 +6158,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="30" hidden="1">
+    <row r="46" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>256</v>
       </c>
@@ -6200,7 +6203,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="30" hidden="1">
+    <row r="47" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>262</v>
       </c>
@@ -6245,7 +6248,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="60" hidden="1">
+    <row r="48" spans="1:18" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>266</v>
       </c>
@@ -6290,7 +6293,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="30" hidden="1">
+    <row r="49" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>270</v>
       </c>
@@ -6335,7 +6338,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="50" spans="1:18" ht="45" hidden="1">
+    <row r="50" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>273</v>
       </c>
@@ -6380,7 +6383,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="60" hidden="1">
+    <row r="51" spans="1:18" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>279</v>
       </c>
@@ -6425,7 +6428,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="45" hidden="1">
+    <row r="52" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>283</v>
       </c>
@@ -6464,7 +6467,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="45" hidden="1">
+    <row r="53" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>287</v>
       </c>
@@ -6509,7 +6512,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="30" hidden="1">
+    <row r="54" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>291</v>
       </c>
@@ -6554,7 +6557,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="55" spans="1:18" ht="30" hidden="1">
+    <row r="55" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>295</v>
       </c>
@@ -6599,7 +6602,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="56" spans="1:18" ht="30" hidden="1">
+    <row r="56" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>301</v>
       </c>
@@ -6644,7 +6647,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="57" spans="1:18" ht="30" hidden="1">
+    <row r="57" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>306</v>
       </c>
@@ -6689,7 +6692,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="58" spans="1:18" ht="30" hidden="1">
+    <row r="58" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>310</v>
       </c>
@@ -6734,7 +6737,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="59" spans="1:18" ht="45" hidden="1">
+    <row r="59" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>315</v>
       </c>
@@ -6779,7 +6782,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="60" spans="1:18" ht="30" hidden="1">
+    <row r="60" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>321</v>
       </c>
@@ -6824,7 +6827,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="61" spans="1:18" ht="60" hidden="1">
+    <row r="61" spans="1:18" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>326</v>
       </c>
@@ -6866,7 +6869,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="45" hidden="1">
+    <row r="62" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>332</v>
       </c>
@@ -6908,7 +6911,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="63" spans="1:18" ht="60" hidden="1">
+    <row r="63" spans="1:18" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>339</v>
       </c>
@@ -6950,7 +6953,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="64" spans="1:18" ht="45" hidden="1">
+    <row r="64" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>345</v>
       </c>
@@ -6986,7 +6989,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="1:18" ht="45" hidden="1">
+    <row r="65" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>349</v>
       </c>
@@ -7028,7 +7031,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="66" spans="1:18" ht="30" hidden="1">
+    <row r="66" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>353</v>
       </c>
@@ -7070,7 +7073,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="67" spans="1:18" ht="45" hidden="1">
+    <row r="67" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>357</v>
       </c>
@@ -7110,7 +7113,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="68" spans="1:18" ht="45" hidden="1">
+    <row r="68" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>360</v>
       </c>
@@ -7149,7 +7152,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="1:18" ht="45" hidden="1">
+    <row r="69" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>367</v>
       </c>
@@ -7188,7 +7191,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="70" spans="1:18" ht="45" hidden="1">
+    <row r="70" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>374</v>
       </c>
@@ -7227,7 +7230,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:18" ht="45" hidden="1">
+    <row r="71" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>377</v>
       </c>
@@ -7266,7 +7269,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:18" ht="45" hidden="1">
+    <row r="72" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>380</v>
       </c>
@@ -7305,7 +7308,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:18" ht="45" hidden="1">
+    <row r="73" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>384</v>
       </c>
@@ -7344,7 +7347,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="74" spans="1:18" ht="45" hidden="1">
+    <row r="74" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>390</v>
       </c>
@@ -7383,7 +7386,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="1:18" ht="45" hidden="1">
+    <row r="75" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>393</v>
       </c>
@@ -7425,7 +7428,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="76" spans="1:18" ht="45" hidden="1">
+    <row r="76" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>397</v>
       </c>
@@ -7464,7 +7467,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="77" spans="1:18" ht="45" hidden="1">
+    <row r="77" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>400</v>
       </c>
@@ -7503,7 +7506,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="78" spans="1:18" ht="45" hidden="1">
+    <row r="78" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>405</v>
       </c>
@@ -7542,7 +7545,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="79" spans="1:18" ht="45" hidden="1">
+    <row r="79" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>409</v>
       </c>
@@ -7581,7 +7584,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="1:18" ht="45" hidden="1">
+    <row r="80" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>413</v>
       </c>
@@ -7620,7 +7623,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="81" spans="1:18" ht="45" hidden="1">
+    <row r="81" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>416</v>
       </c>
@@ -7659,7 +7662,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="82" spans="1:18" ht="45" hidden="1">
+    <row r="82" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>419</v>
       </c>
@@ -7698,7 +7701,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="83" spans="1:18" ht="45" hidden="1">
+    <row r="83" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>422</v>
       </c>
@@ -7737,7 +7740,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="84" spans="1:18" ht="45" hidden="1">
+    <row r="84" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>425</v>
       </c>
@@ -7776,7 +7779,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="85" spans="1:18" ht="45" hidden="1">
+    <row r="85" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>428</v>
       </c>
@@ -7815,7 +7818,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="86" spans="1:18" ht="45" hidden="1">
+    <row r="86" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>432</v>
       </c>
@@ -7854,7 +7857,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="87" spans="1:18" ht="45" hidden="1">
+    <row r="87" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>436</v>
       </c>
@@ -7893,7 +7896,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="88" spans="1:18" ht="45" hidden="1">
+    <row r="88" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>440</v>
       </c>
@@ -7932,7 +7935,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="89" spans="1:18" ht="45" hidden="1">
+    <row r="89" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>444</v>
       </c>
@@ -7971,7 +7974,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="90" spans="1:18" ht="45" hidden="1">
+    <row r="90" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>447</v>
       </c>
@@ -8010,7 +8013,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="91" spans="1:18" ht="45" hidden="1">
+    <row r="91" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>450</v>
       </c>
@@ -8049,7 +8052,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="92" spans="1:18" ht="78.75" hidden="1" customHeight="1">
+    <row r="92" spans="1:18" ht="78.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>455</v>
       </c>
@@ -8088,7 +8091,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="93" spans="1:18" ht="30" hidden="1">
+    <row r="93" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>460</v>
       </c>
@@ -8141,7 +8144,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="94" spans="1:18" ht="60" hidden="1">
+    <row r="94" spans="1:18" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>470</v>
       </c>
@@ -8189,7 +8192,7 @@
       </c>
       <c r="Q94" s="4"/>
     </row>
-    <row r="95" spans="1:18" ht="30" hidden="1">
+    <row r="95" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>475</v>
       </c>
@@ -8239,7 +8242,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="96" spans="1:18" ht="60" hidden="1">
+    <row r="96" spans="1:18" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>480</v>
       </c>
@@ -8287,7 +8290,7 @@
       </c>
       <c r="Q96" s="4"/>
     </row>
-    <row r="97" spans="1:18" ht="30" hidden="1">
+    <row r="97" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>483</v>
       </c>
@@ -8337,7 +8340,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="98" spans="1:18" ht="30" hidden="1">
+    <row r="98" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>489</v>
       </c>
@@ -8387,7 +8390,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="99" spans="1:18" ht="60" hidden="1">
+    <row r="99" spans="1:18" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>492</v>
       </c>
@@ -8440,7 +8443,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="100" spans="1:18" ht="45" hidden="1">
+    <row r="100" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>499</v>
       </c>
@@ -8480,7 +8483,7 @@
       </c>
       <c r="R100" s="4"/>
     </row>
-    <row r="101" spans="1:18" ht="30" hidden="1">
+    <row r="101" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>504</v>
       </c>
@@ -8530,7 +8533,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="102" spans="1:18" ht="45" hidden="1">
+    <row r="102" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>507</v>
       </c>
@@ -8570,7 +8573,7 @@
       </c>
       <c r="R102" s="4"/>
     </row>
-    <row r="103" spans="1:18" ht="30" hidden="1">
+    <row r="103" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>511</v>
       </c>
@@ -8620,7 +8623,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="104" spans="1:18" ht="30" hidden="1">
+    <row r="104" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>514</v>
       </c>
@@ -8670,7 +8673,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="105" spans="1:18" ht="30" hidden="1">
+    <row r="105" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>517</v>
       </c>
@@ -8720,7 +8723,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="106" spans="1:18" ht="45" hidden="1">
+    <row r="106" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>521</v>
       </c>
@@ -8773,7 +8776,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="107" spans="1:18" ht="45" hidden="1">
+    <row r="107" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>525</v>
       </c>
@@ -8826,7 +8829,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="108" spans="1:18" ht="134.25" hidden="1" customHeight="1">
+    <row r="108" spans="1:18" ht="134.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>529</v>
       </c>
@@ -8866,7 +8869,7 @@
       </c>
       <c r="R108" s="4"/>
     </row>
-    <row r="109" spans="1:18" ht="81.75" hidden="1" customHeight="1">
+    <row r="109" spans="1:18" ht="81.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>532</v>
       </c>
@@ -8916,7 +8919,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="110" spans="1:18" ht="60" hidden="1">
+    <row r="110" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>535</v>
       </c>
@@ -8969,7 +8972,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="111" spans="1:18" ht="60" hidden="1" customHeight="1">
+    <row r="111" spans="1:18" ht="60" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>539</v>
       </c>
@@ -9022,7 +9025,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="112" spans="1:18" ht="45" hidden="1">
+    <row r="112" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>545</v>
       </c>
@@ -9075,7 +9078,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="113" spans="1:18" ht="45" hidden="1">
+    <row r="113" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>549</v>
       </c>
@@ -9114,7 +9117,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="114" spans="1:18" ht="30" hidden="1">
+    <row r="114" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>553</v>
       </c>
@@ -9167,7 +9170,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="115" spans="1:18" ht="30" hidden="1">
+    <row r="115" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>557</v>
       </c>
@@ -9220,7 +9223,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="116" spans="1:18" ht="84" hidden="1" customHeight="1">
+    <row r="116" spans="1:18" ht="84" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>563</v>
       </c>
@@ -9273,7 +9276,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="117" spans="1:18" ht="45" hidden="1">
+    <row r="117" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>567</v>
       </c>
@@ -9326,7 +9329,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="118" spans="1:18" ht="45" hidden="1">
+    <row r="118" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>571</v>
       </c>
@@ -9379,7 +9382,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="119" spans="1:18" ht="30" hidden="1">
+    <row r="119" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>574</v>
       </c>
@@ -9432,7 +9435,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="120" spans="1:18" ht="30" hidden="1">
+    <row r="120" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>578</v>
       </c>
@@ -9482,7 +9485,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="121" spans="1:18" ht="30" hidden="1">
+    <row r="121" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>581</v>
       </c>
@@ -9535,7 +9538,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="122" spans="1:18" ht="75" hidden="1">
+    <row r="122" spans="1:18" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>586</v>
       </c>
@@ -9588,7 +9591,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="123" spans="1:18" ht="30" hidden="1">
+    <row r="123" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>591</v>
       </c>
@@ -9638,7 +9641,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="124" spans="1:18" ht="30.75" hidden="1">
+    <row r="124" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>597</v>
       </c>
@@ -9691,7 +9694,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="125" spans="1:18" ht="30">
+    <row r="125" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
         <v>603</v>
       </c>
@@ -9741,7 +9744,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="126" spans="1:18" ht="96.75" hidden="1" customHeight="1">
+    <row r="126" spans="1:18" ht="96.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>608</v>
       </c>
@@ -9794,7 +9797,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="127" spans="1:18" ht="30" hidden="1">
+    <row r="127" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>612</v>
       </c>
@@ -9847,7 +9850,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="128" spans="1:18" ht="30" hidden="1">
+    <row r="128" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
         <v>618</v>
       </c>
@@ -9897,7 +9900,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="129" spans="1:18" ht="45" hidden="1">
+    <row r="129" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
         <v>621</v>
       </c>
@@ -9937,7 +9940,7 @@
       </c>
       <c r="R129" s="4"/>
     </row>
-    <row r="130" spans="1:18" ht="30" hidden="1">
+    <row r="130" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>624</v>
       </c>
@@ -9987,7 +9990,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="131" spans="1:18" ht="30" hidden="1">
+    <row r="131" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
         <v>629</v>
       </c>
@@ -10037,7 +10040,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="132" spans="1:18" ht="45" hidden="1">
+    <row r="132" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
         <v>634</v>
       </c>
@@ -10077,7 +10080,7 @@
       </c>
       <c r="R132" s="4"/>
     </row>
-    <row r="133" spans="1:18" ht="30" hidden="1">
+    <row r="133" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
         <v>639</v>
       </c>
@@ -10127,7 +10130,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="134" spans="1:18" ht="30" hidden="1">
+    <row r="134" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
         <v>643</v>
       </c>
@@ -10177,7 +10180,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="135" spans="1:18" ht="30" hidden="1">
+    <row r="135" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
         <v>646</v>
       </c>
@@ -10227,7 +10230,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="136" spans="1:18" ht="45" hidden="1">
+    <row r="136" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
         <v>649</v>
       </c>
@@ -10280,7 +10283,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="137" spans="1:18" ht="45" hidden="1">
+    <row r="137" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
         <v>655</v>
       </c>
@@ -10320,7 +10323,7 @@
       </c>
       <c r="R137" s="4"/>
     </row>
-    <row r="138" spans="1:18" ht="30" hidden="1">
+    <row r="138" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
         <v>658</v>
       </c>
@@ -10373,7 +10376,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="139" spans="1:18" ht="30" hidden="1">
+    <row r="139" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
         <v>663</v>
       </c>
@@ -10423,7 +10426,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="140" spans="1:18" ht="45" hidden="1">
+    <row r="140" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
         <v>668</v>
       </c>
@@ -10463,7 +10466,7 @@
       </c>
       <c r="R140" s="4"/>
     </row>
-    <row r="141" spans="1:18" ht="30" hidden="1">
+    <row r="141" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
         <v>671</v>
       </c>
@@ -10513,7 +10516,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="142" spans="1:18" ht="30" hidden="1">
+    <row r="142" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
         <v>674</v>
       </c>
@@ -10563,7 +10566,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="143" spans="1:18" ht="30" hidden="1">
+    <row r="143" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
         <v>677</v>
       </c>
@@ -10616,7 +10619,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="144" spans="1:18" ht="30" hidden="1">
+    <row r="144" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
         <v>681</v>
       </c>
@@ -10666,7 +10669,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="145" spans="1:18" ht="89.25" hidden="1" customHeight="1">
+    <row r="145" spans="1:18" ht="89.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
         <v>684</v>
       </c>
@@ -10719,7 +10722,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="146" spans="1:18" ht="45" hidden="1">
+    <row r="146" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
         <v>689</v>
       </c>
@@ -10772,7 +10775,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="147" spans="1:18" ht="75" hidden="1">
+    <row r="147" spans="1:18" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
         <v>693</v>
       </c>
@@ -10825,7 +10828,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="148" spans="1:18" ht="30" hidden="1">
+    <row r="148" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
         <v>698</v>
       </c>
@@ -10875,7 +10878,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="149" spans="1:18" ht="30" hidden="1">
+    <row r="149" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
         <v>701</v>
       </c>
@@ -10925,7 +10928,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="150" spans="1:18" ht="30" hidden="1">
+    <row r="150" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
         <v>704</v>
       </c>
@@ -10975,7 +10978,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="151" spans="1:18" ht="30" hidden="1">
+    <row r="151" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
         <v>707</v>
       </c>
@@ -11028,7 +11031,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="152" spans="1:18" ht="45" hidden="1">
+    <row r="152" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
         <v>711</v>
       </c>
@@ -11068,7 +11071,7 @@
       </c>
       <c r="R152" s="4"/>
     </row>
-    <row r="153" spans="1:18" ht="30" hidden="1">
+    <row r="153" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
         <v>716</v>
       </c>
@@ -11121,7 +11124,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="154" spans="1:18" ht="45" hidden="1">
+    <row r="154" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
         <v>719</v>
       </c>
@@ -11161,7 +11164,7 @@
       </c>
       <c r="R154" s="4"/>
     </row>
-    <row r="155" spans="1:18" ht="45" hidden="1">
+    <row r="155" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
         <v>723</v>
       </c>
@@ -11214,7 +11217,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="156" spans="1:18" ht="30" hidden="1">
+    <row r="156" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
         <v>729</v>
       </c>
@@ -11267,7 +11270,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="157" spans="1:18" ht="30" hidden="1">
+    <row r="157" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
         <v>735</v>
       </c>
@@ -11320,7 +11323,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="158" spans="1:18" ht="60" hidden="1">
+    <row r="158" spans="1:18" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="s">
         <v>739</v>
       </c>
@@ -11370,7 +11373,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="159" spans="1:18" ht="30" hidden="1">
+    <row r="159" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
         <v>742</v>
       </c>
@@ -11423,7 +11426,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="160" spans="1:18" ht="64.5" hidden="1" customHeight="1">
+    <row r="160" spans="1:18" ht="64.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
         <v>747</v>
       </c>
@@ -11473,7 +11476,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="161" spans="1:18" ht="18.75" hidden="1" customHeight="1">
+    <row r="161" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
         <v>751</v>
       </c>
@@ -11513,7 +11516,7 @@
       </c>
       <c r="R161" s="4"/>
     </row>
-    <row r="162" spans="1:18" ht="58.5" hidden="1" customHeight="1">
+    <row r="162" spans="1:18" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
         <v>754</v>
       </c>
@@ -11553,7 +11556,7 @@
       </c>
       <c r="R162" s="4"/>
     </row>
-    <row r="163" spans="1:18" ht="45" hidden="1">
+    <row r="163" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="4" t="s">
         <v>758</v>
       </c>
@@ -11606,7 +11609,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="164" spans="1:18" ht="29.25" hidden="1" customHeight="1">
+    <row r="164" spans="1:18" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
         <v>762</v>
       </c>
@@ -11646,7 +11649,7 @@
       </c>
       <c r="R164" s="4"/>
     </row>
-    <row r="165" spans="1:18" ht="45" hidden="1" customHeight="1">
+    <row r="165" spans="1:18" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
         <v>765</v>
       </c>
@@ -11686,7 +11689,7 @@
       </c>
       <c r="R165" s="4"/>
     </row>
-    <row r="166" spans="1:18" ht="60" hidden="1">
+    <row r="166" spans="1:18" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="4" t="s">
         <v>768</v>
       </c>
@@ -11739,7 +11742,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="167" spans="1:18" ht="45" hidden="1">
+    <row r="167" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
         <v>772</v>
       </c>
@@ -11792,7 +11795,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="168" spans="1:18" ht="30" hidden="1">
+    <row r="168" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
         <v>776</v>
       </c>
@@ -11842,7 +11845,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="169" spans="1:18" ht="45" hidden="1">
+    <row r="169" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
         <v>779</v>
       </c>
@@ -11882,7 +11885,7 @@
       </c>
       <c r="R169" s="4"/>
     </row>
-    <row r="170" spans="1:18" ht="30" hidden="1">
+    <row r="170" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
         <v>782</v>
       </c>
@@ -11932,7 +11935,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="171" spans="1:18" ht="45" hidden="1">
+    <row r="171" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
         <v>786</v>
       </c>
@@ -11972,7 +11975,7 @@
       </c>
       <c r="R171" s="4"/>
     </row>
-    <row r="172" spans="1:18" ht="30" hidden="1">
+    <row r="172" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
         <v>789</v>
       </c>
@@ -12022,7 +12025,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="173" spans="1:18" ht="30" hidden="1">
+    <row r="173" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="4" t="s">
         <v>794</v>
       </c>
@@ -12072,7 +12075,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="174" spans="1:18" ht="45" hidden="1">
+    <row r="174" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
         <v>797</v>
       </c>
@@ -12112,7 +12115,7 @@
       </c>
       <c r="R174" s="4"/>
     </row>
-    <row r="175" spans="1:18" ht="31.5" hidden="1" customHeight="1">
+    <row r="175" spans="1:18" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="4" t="s">
         <v>800</v>
       </c>
@@ -12165,7 +12168,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="176" spans="1:18" ht="30" hidden="1">
+    <row r="176" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="s">
         <v>804</v>
       </c>
@@ -12215,7 +12218,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="177" spans="1:18" ht="30" hidden="1">
+    <row r="177" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="4" t="s">
         <v>808</v>
       </c>
@@ -12265,7 +12268,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="178" spans="1:18" ht="32.25" hidden="1" customHeight="1">
+    <row r="178" spans="1:18" ht="32.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="4" t="s">
         <v>811</v>
       </c>
@@ -12315,7 +12318,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="179" spans="1:18" ht="45" hidden="1">
+    <row r="179" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="4" t="s">
         <v>815</v>
       </c>
@@ -12355,7 +12358,7 @@
       </c>
       <c r="R179" s="4"/>
     </row>
-    <row r="180" spans="1:18" ht="45" hidden="1">
+    <row r="180" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="4" t="s">
         <v>819</v>
       </c>
@@ -12395,7 +12398,7 @@
       </c>
       <c r="R180" s="4"/>
     </row>
-    <row r="181" spans="1:18" ht="45" hidden="1">
+    <row r="181" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="4" t="s">
         <v>822</v>
       </c>
@@ -12435,7 +12438,7 @@
       </c>
       <c r="R181" s="4"/>
     </row>
-    <row r="182" spans="1:18" ht="60" hidden="1">
+    <row r="182" spans="1:18" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="4" t="s">
         <v>825</v>
       </c>
@@ -12488,7 +12491,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="183" spans="1:18" ht="60" hidden="1">
+    <row r="183" spans="1:18" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="4" t="s">
         <v>829</v>
       </c>
@@ -12541,7 +12544,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="184" spans="1:18" ht="39.75" hidden="1" customHeight="1">
+    <row r="184" spans="1:18" ht="39.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="4" t="s">
         <v>834</v>
       </c>
@@ -12594,7 +12597,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="185" spans="1:18" ht="30" hidden="1">
+    <row r="185" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="4" t="s">
         <v>840</v>
       </c>
@@ -12647,7 +12650,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="186" spans="1:18" ht="45" hidden="1">
+    <row r="186" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="4" t="s">
         <v>845</v>
       </c>
@@ -12700,7 +12703,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="187" spans="1:18" ht="30" hidden="1">
+    <row r="187" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="4" t="s">
         <v>849</v>
       </c>
@@ -12750,7 +12753,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="188" spans="1:18" ht="45" hidden="1">
+    <row r="188" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="4" t="s">
         <v>854</v>
       </c>
@@ -12803,7 +12806,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="189" spans="1:18" ht="45" hidden="1">
+    <row r="189" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="4" t="s">
         <v>858</v>
       </c>
@@ -12842,7 +12845,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="190" spans="1:18" ht="45" hidden="1">
+    <row r="190" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="4" t="s">
         <v>861</v>
       </c>
@@ -12881,7 +12884,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="191" spans="1:18" ht="45" hidden="1">
+    <row r="191" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="4" t="s">
         <v>865</v>
       </c>
@@ -12920,7 +12923,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="192" spans="1:18" ht="45" hidden="1">
+    <row r="192" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="4" t="s">
         <v>869</v>
       </c>
@@ -12959,7 +12962,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="193" spans="1:18" ht="45" hidden="1">
+    <row r="193" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="4" t="s">
         <v>872</v>
       </c>
@@ -12998,7 +13001,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="194" spans="1:18" ht="45" hidden="1">
+    <row r="194" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="4" t="s">
         <v>877</v>
       </c>
@@ -13037,7 +13040,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="195" spans="1:18" ht="30" hidden="1">
+    <row r="195" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="4" t="s">
         <v>880</v>
       </c>
@@ -13087,7 +13090,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="196" spans="1:18" ht="30" hidden="1">
+    <row r="196" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="4" t="s">
         <v>883</v>
       </c>
@@ -13140,7 +13143,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="197" spans="1:18" ht="45" hidden="1">
+    <row r="197" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="4" t="s">
         <v>887</v>
       </c>
@@ -13180,7 +13183,7 @@
       </c>
       <c r="R197" s="4"/>
     </row>
-    <row r="198" spans="1:18" ht="30" hidden="1">
+    <row r="198" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="4" t="s">
         <v>890</v>
       </c>
@@ -13233,7 +13236,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="199" spans="1:18" ht="45" hidden="1">
+    <row r="199" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="4" t="s">
         <v>894</v>
       </c>
@@ -13273,7 +13276,7 @@
       </c>
       <c r="R199" s="4"/>
     </row>
-    <row r="200" spans="1:18" ht="30" hidden="1">
+    <row r="200" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="4" t="s">
         <v>897</v>
       </c>
@@ -13326,7 +13329,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="201" spans="1:18" ht="45" hidden="1">
+    <row r="201" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="4" t="s">
         <v>901</v>
       </c>
@@ -13366,7 +13369,7 @@
       </c>
       <c r="R201" s="4"/>
     </row>
-    <row r="202" spans="1:18" ht="30" hidden="1">
+    <row r="202" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="4" t="s">
         <v>904</v>
       </c>
@@ -13419,7 +13422,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="203" spans="1:18" ht="75" hidden="1">
+    <row r="203" spans="1:18" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="4" t="s">
         <v>907</v>
       </c>
@@ -13472,7 +13475,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="204" spans="1:18" ht="45" hidden="1">
+    <row r="204" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="4" t="s">
         <v>911</v>
       </c>
@@ -13514,7 +13517,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="205" spans="1:18" ht="38.25" hidden="1" customHeight="1">
+    <row r="205" spans="1:18" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="4" t="s">
         <v>915</v>
       </c>
@@ -13567,7 +13570,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="206" spans="1:18" ht="45" hidden="1">
+    <row r="206" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="4" t="s">
         <v>920</v>
       </c>
@@ -13607,7 +13610,7 @@
       </c>
       <c r="R206" s="4"/>
     </row>
-    <row r="207" spans="1:18" ht="45" hidden="1">
+    <row r="207" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="4" t="s">
         <v>924</v>
       </c>
@@ -13647,7 +13650,7 @@
       </c>
       <c r="R207" s="4"/>
     </row>
-    <row r="208" spans="1:18" ht="45" hidden="1">
+    <row r="208" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="4" t="s">
         <v>927</v>
       </c>
@@ -13687,7 +13690,7 @@
       </c>
       <c r="R208" s="4"/>
     </row>
-    <row r="209" spans="1:18" ht="45" hidden="1">
+    <row r="209" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="4" t="s">
         <v>931</v>
       </c>
@@ -13727,7 +13730,7 @@
       </c>
       <c r="R209" s="4"/>
     </row>
-    <row r="210" spans="1:18" ht="60" hidden="1">
+    <row r="210" spans="1:18" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="4" t="s">
         <v>934</v>
       </c>
@@ -13780,7 +13783,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="211" spans="1:18" ht="60" hidden="1">
+    <row r="211" spans="1:18" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="4" t="s">
         <v>940</v>
       </c>
@@ -13830,7 +13833,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="212" spans="1:18" ht="45" hidden="1">
+    <row r="212" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="4" t="s">
         <v>943</v>
       </c>
@@ -13870,7 +13873,7 @@
       </c>
       <c r="R212" s="4"/>
     </row>
-    <row r="213" spans="1:18" ht="45" hidden="1">
+    <row r="213" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="4" t="s">
         <v>946</v>
       </c>
@@ -13923,7 +13926,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="214" spans="1:18" ht="30" hidden="1">
+    <row r="214" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="4" t="s">
         <v>950</v>
       </c>
@@ -13976,7 +13979,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="215" spans="1:18" ht="58.5" hidden="1" customHeight="1">
+    <row r="215" spans="1:18" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="4" t="s">
         <v>954</v>
       </c>
@@ -14029,7 +14032,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="216" spans="1:18" ht="45" hidden="1">
+    <row r="216" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="4" t="s">
         <v>959</v>
       </c>
@@ -14068,7 +14071,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="217" spans="1:18" ht="45" hidden="1">
+    <row r="217" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="4" t="s">
         <v>962</v>
       </c>
@@ -14107,7 +14110,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="218" spans="1:18" ht="45" hidden="1">
+    <row r="218" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="4" t="s">
         <v>962</v>
       </c>
@@ -14146,7 +14149,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="219" spans="1:18" ht="45" hidden="1">
+    <row r="219" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="4" t="s">
         <v>962</v>
       </c>
@@ -14185,7 +14188,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="220" spans="1:18" ht="45" hidden="1">
+    <row r="220" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="4" t="s">
         <v>969</v>
       </c>
@@ -14224,7 +14227,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="221" spans="1:18" ht="45" hidden="1">
+    <row r="221" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="4" t="s">
         <v>969</v>
       </c>
@@ -14263,7 +14266,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="222" spans="1:18" ht="45" hidden="1">
+    <row r="222" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="4" t="s">
         <v>976</v>
       </c>
@@ -14302,7 +14305,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="223" spans="1:18" ht="45" hidden="1">
+    <row r="223" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="4" t="s">
         <v>976</v>
       </c>
@@ -14341,31 +14344,31 @@
         <v>70</v>
       </c>
     </row>
-    <row r="224" spans="1:18" hidden="1">
+    <row r="224" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="L224" s="5"/>
       <c r="P224" s="4"/>
     </row>
-    <row r="225" spans="12:16" hidden="1">
+    <row r="225" spans="12:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="L225" s="5"/>
       <c r="P225" s="4"/>
     </row>
-    <row r="226" spans="12:16" hidden="1">
+    <row r="226" spans="12:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="L226" s="5"/>
       <c r="P226" s="4"/>
     </row>
-    <row r="227" spans="12:16" hidden="1">
+    <row r="227" spans="12:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="L227" s="5"/>
       <c r="P227" s="4"/>
     </row>
-    <row r="228" spans="12:16" hidden="1">
+    <row r="228" spans="12:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="L228" s="5"/>
       <c r="P228" s="4"/>
     </row>
-    <row r="229" spans="12:16" hidden="1">
+    <row r="229" spans="12:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="L229" s="5"/>
       <c r="P229" s="4"/>
     </row>
-    <row r="230" spans="12:16" hidden="1">
+    <row r="230" spans="12:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="L230" s="5"/>
       <c r="P230" s="4"/>
     </row>
@@ -14429,7 +14432,7 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59.140625" customWidth="1"/>
     <col min="2" max="2" width="75.140625" customWidth="1"/>
@@ -14437,7 +14440,7 @@
     <col min="4" max="4" width="34" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>981</v>
       </c>
@@ -14451,7 +14454,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -14465,7 +14468,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -14479,7 +14482,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="35.25" customHeight="1">
+    <row r="4" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -14493,7 +14496,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="34.5" customHeight="1">
+    <row r="5" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -14507,7 +14510,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -14521,7 +14524,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>77</v>
       </c>
@@ -14532,7 +14535,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>68</v>
       </c>
@@ -14540,7 +14543,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>109</v>
       </c>
@@ -14548,17 +14551,17 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="2:2">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>987</v>
       </c>
@@ -14576,14 +14579,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b355cb27-d675-450b-9661-86e24d269bf4" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a6a2b1f6-3df7-4aa2-8f71-3c19eb8f1b77">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14816,22 +14817,50 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b355cb27-d675-450b-9661-86e24d269bf4" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a6a2b1f6-3df7-4aa2-8f71-3c19eb8f1b77">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCB942B1-15F9-46BE-9AEF-1CA00CCEC400}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94B4DD76-D2A0-4C43-8485-C3BF2C1BE59B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23EF927E-CA1A-4920-B4B7-C60779EC76E1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23EF927E-CA1A-4920-B4B7-C60779EC76E1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a6a2b1f6-3df7-4aa2-8f71-3c19eb8f1b77"/>
+    <ds:schemaRef ds:uri="b355cb27-d675-450b-9661-86e24d269bf4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94B4DD76-D2A0-4C43-8485-C3BF2C1BE59B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCB942B1-15F9-46BE-9AEF-1CA00CCEC400}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b355cb27-d675-450b-9661-86e24d269bf4"/>
+    <ds:schemaRef ds:uri="a6a2b1f6-3df7-4aa2-8f71-3c19eb8f1b77"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>